<commit_message>
Created meet visualization and tabulation functions.
</commit_message>
<xml_diff>
--- a/meetResultsGirls2025.xlsx
+++ b/meetResultsGirls2025.xlsx
@@ -440,12 +440,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>meetID</t>
+          <t>SheetName</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>raceID</t>
+          <t>MeetTitle</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -472,12 +472,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>m250816-light-up-the-night</t>
+          <t>light-up-the-nightGirlsVarsity</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>f3000mfinalsFinals99</t>
+          <t>light-up-the-night</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -502,12 +502,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>m250816-light-up-the-night</t>
+          <t>light-up-the-nightGirlsJV</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>f3000mfinalsFinalsOpen</t>
+          <t>light-up-the-night</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -532,12 +532,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>m250823-fightertown-xc-invitational</t>
+          <t>fightertown-xc-invitationalGirlsJV</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>f4000mfinalsFinals</t>
+          <t>fightertown-xc-invitational</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -562,12 +562,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>m250823-fightertown-xc-invitational</t>
+          <t>fightertown-xc-invitationalGirlsVarsity</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>f5000mfinalsFinals</t>
+          <t>fightertown-xc-invitational</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -7582,7 +7582,7 @@
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Valeria Valdivia</t>
+          <t>Valerie Valdivia</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">

</xml_diff>